<commit_message>
all crud scenarios working
</commit_message>
<xml_diff>
--- a/bugs.xlsx
+++ b/bugs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Documents\VSCode\backbase_tech_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E191A2E-7C49-4183-8E98-D11A797FC113}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CF9421-1CE9-4C68-9F0E-032AE35AB59B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{19FD1596-77E6-4FBC-A324-70595D067C3A}"/>
+    <workbookView xWindow="3855" yWindow="3855" windowWidth="18900" windowHeight="11055" xr2:uid="{19FD1596-77E6-4FBC-A324-70595D067C3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Bugs</t>
   </si>
@@ -44,7 +44,44 @@
     <t>Outcome</t>
   </si>
   <si>
-    <t>Deleted computer doesn't display name</t>
+    <t>Can't search with $ in the name</t>
+  </si>
+  <si>
+    <t>Pagination broken</t>
+  </si>
+  <si>
+    <t>1. search 'z'
+2. go to next page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">displays 11 to 20 out of 14. Before clicking next it displays 1 - 10 of 24 </t>
+  </si>
+  <si>
+    <t>Deleted computer confirmation message doesn't display name</t>
+  </si>
+  <si>
+    <t>Able to set dates in future</t>
+  </si>
+  <si>
+    <t>Able to set dates  from far in the past</t>
+  </si>
+  <si>
+    <t>Date error -  ('yyyy-MM-dd') - Inconsistent case</t>
+  </si>
+  <si>
+    <t>Cannot easily navigate to first and last pages of computer list</t>
+  </si>
+  <si>
+    <t>Deleting a computer from search returns you to page 1 and clears search</t>
+  </si>
+  <si>
+    <t>When reloading page or adding new computer occasionally the page styling isn't visible for a split second</t>
+  </si>
+  <si>
+    <t>Errors when setting fields on add/edit computer don't inform you of the error</t>
+  </si>
+  <si>
+    <t>Able to add computers where the discontinued date is before the introduced date.</t>
   </si>
 </sst>
 </file>
@@ -80,13 +117,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -100,14 +159,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6572E1CB-32D3-45AA-BEE1-3B5078412905}" name="Table1" displayName="Table1" ref="A3:C4" totalsRowShown="0">
-  <autoFilter ref="A3:C4" xr:uid="{2ED82F8D-E1C1-4F16-8BE6-69DF9CA83C3A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6572E1CB-32D3-45AA-BEE1-3B5078412905}" name="Table1" displayName="Table1" ref="A3:C14" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="A3:C14" xr:uid="{2ED82F8D-E1C1-4F16-8BE6-69DF9CA83C3A}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{F7789E19-8E56-4615-9813-FF03F8C49304}" name="Description"/>
-    <tableColumn id="2" xr3:uid="{53FECECB-AD21-47AA-AA6A-E824C8F20925}" name="Steps"/>
-    <tableColumn id="3" xr3:uid="{764599BC-2976-4481-A5AF-E8CC507D4E87}" name="Outcome"/>
+    <tableColumn id="1" xr3:uid="{F7789E19-8E56-4615-9813-FF03F8C49304}" name="Description" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{53FECECB-AD21-47AA-AA6A-E824C8F20925}" name="Steps" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{764599BC-2976-4481-A5AF-E8CC507D4E87}" name="Outcome" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -408,26 +467,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44CB0688-3BC8-4498-9E4A-78EF0AF6A981}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="63.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -437,15 +496,92 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
all tests added, working tests passing. Readme updated
</commit_message>
<xml_diff>
--- a/bugs.xlsx
+++ b/bugs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Documents\VSCode\backbase_tech_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CF9421-1CE9-4C68-9F0E-032AE35AB59B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43488F8F-571C-477E-BB2F-71B25950256E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="18900" windowHeight="11055" xr2:uid="{19FD1596-77E6-4FBC-A324-70595D067C3A}"/>
+    <workbookView xWindow="10635" yWindow="3615" windowWidth="18900" windowHeight="11055" xr2:uid="{19FD1596-77E6-4FBC-A324-70595D067C3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
   <si>
     <t>Bugs</t>
   </si>
@@ -42,33 +42,15 @@
   </si>
   <si>
     <t>Outcome</t>
-  </si>
-  <si>
-    <t>Can't search with $ in the name</t>
-  </si>
-  <si>
-    <t>Pagination broken</t>
   </si>
   <si>
     <t>1. search 'z'
 2. go to next page</t>
   </si>
   <si>
-    <t xml:space="preserve">displays 11 to 20 out of 14. Before clicking next it displays 1 - 10 of 24 </t>
-  </si>
-  <si>
     <t>Deleted computer confirmation message doesn't display name</t>
   </si>
   <si>
-    <t>Able to set dates in future</t>
-  </si>
-  <si>
-    <t>Able to set dates  from far in the past</t>
-  </si>
-  <si>
-    <t>Date error -  ('yyyy-MM-dd') - Inconsistent case</t>
-  </si>
-  <si>
     <t>Cannot easily navigate to first and last pages of computer list</t>
   </si>
   <si>
@@ -82,14 +64,214 @@
   </si>
   <si>
     <t>Able to add computers where the discontinued date is before the introduced date.</t>
+  </si>
+  <si>
+    <t>Pagination displays incorrectly</t>
+  </si>
+  <si>
+    <t>1. Add a computer
+2. Delete computer</t>
+  </si>
+  <si>
+    <t>Message displays ' Done! Computer has been deleted ' but not what computer you deleted</t>
+  </si>
+  <si>
+    <t>Can't search with symbols in the name</t>
+  </si>
+  <si>
+    <t>1. Add a computer with name" AAA !!""££$$%^^&amp;&amp;**(())__++--==0987654321[]{}:;@'~#/?.,&lt;&gt;|`¬"
+2. Search for computer</t>
+  </si>
+  <si>
+    <t>1. Add or update a computer
+2. Either in the discontinued or introduced fields set the date to something like 9999-12-12
+3. Add/Save computer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Displays 11 to 20 out of 14. Before clicking next it displays 1 - 10 of 24 </t>
+  </si>
+  <si>
+    <t>Computer add/updated with date</t>
+  </si>
+  <si>
+    <t>1. Add or update a computer
+2. Either in the discontinued or introduced fields set the date to something like 1066-12-12
+3. Add/Save computer</t>
+  </si>
+  <si>
+    <t>No validation on date input allowing you to add dates in the future.</t>
+  </si>
+  <si>
+    <t>1. Add or update a computer</t>
+  </si>
+  <si>
+    <t>Next to the date fields, the date format has lower cas yyyy and dd but upper case MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ('yyyy-MM-dd') - Inconsistent case for date format</t>
+  </si>
+  <si>
+    <t>1. Navigate to last page of computers</t>
+  </si>
+  <si>
+    <t>You need to click next 58 ~ times</t>
+  </si>
+  <si>
+    <t>1. Search for a computer
+2. Delete computer</t>
+  </si>
+  <si>
+    <t>When you delete you are returned to page one of computer results instead of filtered results.</t>
+  </si>
+  <si>
+    <t>1. Hit refresh multiple times</t>
+  </si>
+  <si>
+    <t>If you watch carefully occasionalyl the styling isn't present.</t>
+  </si>
+  <si>
+    <t>1. Create/updatea computer
+2. Delete name so there is no name
+3. Add/Save
+4. Repeat with invalid dates such as 'date' or '1999-99-99'</t>
+  </si>
+  <si>
+    <t>The page errors but there is no information on why.</t>
+  </si>
+  <si>
+    <t>1. Add or update a computer
+2 .In the discontinued field set the date to 2009-12-12
+3. In the Introducedd field set the date to 2019-12-12
+3. Add/Save computer</t>
+  </si>
+  <si>
+    <t>Computer will be added with dates that make no sense.</t>
+  </si>
+  <si>
+    <t>Able to add computers without a company or date</t>
+  </si>
+  <si>
+    <t>1. Add or update a computer
+2 .Enter only a name
+3. Click add/save</t>
+  </si>
+  <si>
+    <t>Computer will be added without dates or company</t>
+  </si>
+  <si>
+    <t>Unable to add new companies</t>
+  </si>
+  <si>
+    <t>1. Add or update a computer
+2. Try to add a new company</t>
+  </si>
+  <si>
+    <t>There is no way to add a new company or indicate that the company for the computer isn't listed.</t>
+  </si>
+  <si>
+    <t>Company list isn't ordered</t>
+  </si>
+  <si>
+    <t>1. Add or update a computer
+2. Open company list and view order</t>
+  </si>
+  <si>
+    <t>The ordering isn't alphabetical and seems a bit random.</t>
+  </si>
+  <si>
+    <t>URL hacking not handled</t>
+  </si>
+  <si>
+    <t>1. Change the url to something like 'computer-database.herokuapp.com/computers/delete' and hit enter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You get a brown header with bad request. </t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Any user can access the page</t>
+  </si>
+  <si>
+    <t>No Authentication</t>
+  </si>
+  <si>
+    <t>API doesn't require a key</t>
+  </si>
+  <si>
+    <t>1. Create a post request in a tool such as postman with:
+- Endpoint - http://computer-database.herokuapp.com/computers
+Body:
+- name:test
+- introduced:2009-05-01
+- discontinued:2019-05-01
+- company:1</t>
+  </si>
+  <si>
+    <t>Computer is added. This also applies to deleting.</t>
+  </si>
+  <si>
+    <t>Unable to search by date or company</t>
+  </si>
+  <si>
+    <t>1. perform search for a computer where you know the date or company</t>
+  </si>
+  <si>
+    <t>Search does not return any results.</t>
+  </si>
+  <si>
+    <t>Search does not return correct results.</t>
+  </si>
+  <si>
+    <t>No confirmation when deleting computer</t>
+  </si>
+  <si>
+    <t>1. Delete computer</t>
+  </si>
+  <si>
+    <t>There is no confirmation of 'Are you sure? Yes/no' when you delete a computer</t>
+  </si>
+  <si>
+    <t>Long computer names overlap success container</t>
+  </si>
+  <si>
+    <t>1. Add a computer that has a name with around 1000 characters.</t>
+  </si>
+  <si>
+    <t>Computer name overlaps success container</t>
+  </si>
+  <si>
+    <t>Long computer names are nto truncated</t>
+  </si>
+  <si>
+    <t>Computer name causes the table to increase in size so you need to scrol to see date and company.</t>
+  </si>
+  <si>
+    <t>Company with value 21 missing from company select</t>
+  </si>
+  <si>
+    <t>1. Open developer console
+2. Inspect company list on the add/edit computer screen.</t>
+  </si>
+  <si>
+    <t>If you go through all the companies, company with value 21 is missing.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -123,21 +305,30 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -159,12 +350,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6572E1CB-32D3-45AA-BEE1-3B5078412905}" name="Table1" displayName="Table1" ref="A3:C14" totalsRowShown="0" dataDxfId="3">
-  <autoFilter ref="A3:C14" xr:uid="{2ED82F8D-E1C1-4F16-8BE6-69DF9CA83C3A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6572E1CB-32D3-45AA-BEE1-3B5078412905}" name="Table1" displayName="Table1" ref="A3:C25" dataDxfId="6">
+  <autoFilter ref="A3:C25" xr:uid="{2ED82F8D-E1C1-4F16-8BE6-69DF9CA83C3A}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{F7789E19-8E56-4615-9813-FF03F8C49304}" name="Description" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{53FECECB-AD21-47AA-AA6A-E824C8F20925}" name="Steps" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{764599BC-2976-4481-A5AF-E8CC507D4E87}" name="Outcome" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{F7789E19-8E56-4615-9813-FF03F8C49304}" name="Description" totalsRowLabel="Total" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{53FECECB-AD21-47AA-AA6A-E824C8F20925}" name="Steps" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{764599BC-2976-4481-A5AF-E8CC507D4E87}" name="Outcome" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -467,21 +658,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44CB0688-3BC8-4498-9E4A-78EF0AF6A981}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
-    <col min="3" max="3" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="63.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -489,93 +680,254 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="B14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="B15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>